<commit_message>
classify mutants, create chart, minor cleanups
</commit_message>
<xml_diff>
--- a/casestudy/memfs-853/results.xlsx
+++ b/casestudy/memfs-853/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franktip/git/mutation-testing-data/casestudy/memfs-853/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991274F4-9324-D64E-8F71-68083901C15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C77732-9420-A14D-A777-E28D5301AF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="7400" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{BA8F4140-1AF3-1848-B3E0-7ADBCED5078A}"/>
+    <workbookView xWindow="7360" yWindow="7400" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{BA8F4140-1AF3-1848-B3E0-7ADBCED5078A}"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="6" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <t>68 test failures, all different</t>
   </si>
   <si>
-    <t>86 test failures</t>
-  </si>
-  <si>
     <t>see file</t>
   </si>
   <si>
@@ -658,6 +655,9 @@
   </si>
   <si>
     <t>surviving mutant -- same behavior as the fixed version</t>
+  </si>
+  <si>
+    <t>86 test failures, including the test failures caused by the original bug</t>
   </si>
 </sst>
 </file>
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9638C49-8A1E-0246-BFEE-36B6AD226B87}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45260694-0BBD-5143-B71E-4CB7D6F62B75}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" activeCellId="1" sqref="B8 C8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1162,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>29</v>
@@ -1174,7 +1174,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
@@ -1185,10 +1185,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1196,10 +1196,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1207,10 +1207,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1229,10 +1229,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1240,10 +1240,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1251,10 +1251,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1262,10 +1262,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1273,10 +1273,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1284,10 +1284,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="238" x14ac:dyDescent="0.2">
@@ -1306,10 +1306,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="238" x14ac:dyDescent="0.2">
@@ -1317,10 +1317,10 @@
         <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C430C8-EF7C-864F-9C13-90FBBD429C35}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
@@ -1360,7 +1360,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1368,22 +1368,22 @@
         <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1391,15 +1391,15 @@
         <v>14</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -1413,10 +1413,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1424,10 +1424,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1446,21 +1446,21 @@
         <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1468,10 +1468,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1479,10 +1479,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1490,15 +1490,15 @@
         <v>24</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
@@ -1509,24 +1509,24 @@
     </row>
     <row r="15" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="238" x14ac:dyDescent="0.2">
@@ -1534,10 +1534,10 @@
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1581,36 +1581,36 @@
     </row>
     <row r="2" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1618,10 +1618,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1629,10 +1629,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1651,21 +1651,21 @@
         <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1673,10 +1673,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1684,10 +1684,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1695,10 +1695,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1706,10 +1706,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="238" x14ac:dyDescent="0.2">
@@ -1725,24 +1725,24 @@
     </row>
     <row r="15" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1789,22 +1789,22 @@
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1812,10 +1812,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1823,21 +1823,21 @@
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1856,21 +1856,21 @@
         <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1878,10 +1878,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1889,10 +1889,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -1900,32 +1900,32 @@
         <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="238" x14ac:dyDescent="0.2">
@@ -1933,10 +1933,10 @@
         <v>28</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="238" x14ac:dyDescent="0.2">
@@ -1944,10 +1944,10 @@
         <v>27</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1986,7 +1986,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="218" customHeight="1" x14ac:dyDescent="0.2">
@@ -1994,10 +1994,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -2006,24 +2006,24 @@
         <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -2031,10 +2031,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -2042,15 +2042,15 @@
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>0</v>
@@ -2061,24 +2061,24 @@
     </row>
     <row r="8" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -2086,10 +2086,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -2097,21 +2097,21 @@
         <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.2">
@@ -2119,43 +2119,43 @@
         <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>